<commit_message>
Formula corrections in "ASVS results" tab
Several fields in the ASVS results didn't include the last criteria.
Architecture read B2:B11, which is only 10 criterias, missing line 12.
This PR fixes these issues for Architecture, Authentication,
Error handling and Logging and Configuration.
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e/source/github.com/emilva/owasp-asvs-checklist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stalepettersen/git/external/owasp-asvs-checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="620" windowWidth="43260" windowHeight="22900" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -1785,11 +1785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-928214896"/>
-        <c:axId val="-928212576"/>
+        <c:axId val="849569552"/>
+        <c:axId val="709035664"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-928214896"/>
+        <c:axId val="849569552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,7 +1800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-928212576"/>
+        <c:crossAx val="709035664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1808,7 +1808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-928212576"/>
+        <c:axId val="709035664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1819,7 +1819,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-928214896"/>
+        <c:crossAx val="849569552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2200,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2235,12 +2235,12 @@
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <f>0+COUNTIF(Architecture!D2:D11,"Valid")</f>
+        <f>0+COUNTIF(Architecture!D2:D12,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <f>COUNTIF(Architecture!D2:D11,"&lt;&gt;Not Applicable")</f>
-        <v>10</v>
+        <f>COUNTIF(Architecture!D2:D12,"&lt;&gt;Not Applicable")</f>
+        <v>11</v>
       </c>
       <c r="D2" s="6">
         <f t="shared" ref="D2:D17" si="0">(B2/C2)*100</f>
@@ -2253,12 +2253,12 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <f>COUNTIF(Authentication!D2:D27,"Valid")</f>
+        <f>COUNTIF(Authentication!D2:D28,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C3" s="8">
-        <f>COUNTIF(Authentication!D2:D27,"&lt;&gt;Not Applicable")</f>
-        <v>26</v>
+        <f>COUNTIF(Authentication!D2:D28,"&lt;&gt;Not Applicable")</f>
+        <v>27</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" si="0"/>
@@ -2344,7 +2344,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="8">
-        <f>COUNTIF('Error Handling and Logging'!D2:D13,"Valid")</f>
+        <f>COUNTIF('Error Handling and Logging'!D2:D14,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C8" s="8">
@@ -2506,12 +2506,12 @@
         <v>20</v>
       </c>
       <c r="B17" s="5">
-        <f>COUNTIF(Configuration!D2:D10,"Valid")</f>
+        <f>COUNTIF(Configuration!D2:D11,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C17" s="8">
-        <f>COUNTIF(Configuration!D2:D10,"&lt;&gt;Not Applicable")</f>
-        <v>9</v>
+        <f>COUNTIF(Configuration!D2:D11,"&lt;&gt;Not Applicable")</f>
+        <v>10</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
@@ -3919,8 +3919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4111,10 +4111,11 @@
       <c r="C12" s="14" t="s">
         <v>368</v>
       </c>
+      <c r="D12" s="15"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4131,7 +4132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -5430,7 +5431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>